<commit_message>
excel a punto de terminar
</commit_message>
<xml_diff>
--- a/02-session/Thesaurus.xlsx
+++ b/02-session/Thesaurus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aprendiz\Downloads\ADSO-2901817\02-session\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b965202a72a8c85f/Desktop/ADSO-2901817/02-session/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AD53B7-D982-4044-9425-B2FEBCB06AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{12AD53B7-D982-4044-9425-B2FEBCB06AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB25F187-ED11-4368-8505-8D64B513974F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{CBF535E4-71E5-47C2-9BF5-65E8EF8C5F03}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="20790" windowHeight="15585" activeTab="3" xr2:uid="{CBF535E4-71E5-47C2-9BF5-65E8EF8C5F03}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="327">
   <si>
     <t>Término o Frase</t>
   </si>
@@ -977,6 +977,55 @@
   </si>
   <si>
     <t>https://www.investigarmqr.com/ojs/index.php/mqr/article/view/886/3451</t>
+  </si>
+  <si>
+    <t>patrones de diseño software "colombia"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIVERSIDAD COOPERATIVA DE COLOMBIA RUTA DE CLASE N0.3: Patrones de Diseño. </t>
+  </si>
+  <si>
+    <t>https://repository.ucc.edu.co/bitstreams/fddbdcca-805f-4384-a6f4-be5ca3fed330/download</t>
+  </si>
+  <si>
+    <t>Patrones de Diseño Refactorización y Antipatrones Ventajas y Desventajas de su Utilización en el Software Orientado a Objetos</t>
+  </si>
+  <si>
+    <t>https://revistas.ucasal.edu.ar/index.php/CI/article/view/178?utm_source=chatgpt.com</t>
+  </si>
+  <si>
+    <t>Patrones   de   Diseño,   Refactorización   y   Antipatrones.   Ventajas  y  Desventajas  de  su  Utilización  en  el  Software  Orientado a Objetos</t>
+  </si>
+  <si>
+    <t>https://bibliotecas.ucasal.edu.ar/opac_css/index.php?lvl=cmspage&amp;pageid=24&amp;id_notice=60533</t>
+  </si>
+  <si>
+    <t>Patrones de diseño, refactorización y antipatrones : Ventajas y desventajas de su utilización en el software orientado a objetos</t>
+  </si>
+  <si>
+    <t>Patrones y Antipatrones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METODOLOGÍA PARA EL REUSO EFECTIVO DE PATRONES DE REQUISITOS EN LA INGENIERÍA DE SOFTWARE </t>
+  </si>
+  <si>
+    <t>https://dspace.tdea.edu.co/entities/publication/c9505ba8-56dc-4c96-83c7-56df101e1ab8</t>
+  </si>
+  <si>
+    <t>antipatrones desarrollo de software "articulos "</t>
+  </si>
+  <si>
+    <t>https://osgg.net/omarsite/resources/papers/ev_arch_02.pdf</t>
+  </si>
+  <si>
+    <t>Evaluando la arquitectura de software</t>
+  </si>
+  <si>
+    <t>Modelo Teórico para la Identificacion del Antipatron
+"Stovepipe System " en la Etapa de la Implementacion de una Arquitectura de Software</t>
+  </si>
+  <si>
+    <t>http://revistasbolivianas.umsa.bo/scielo.php?pid=S3333-77772014000100023&amp;script=sci_arttext&amp;tlng=es</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1361,11 +1410,35 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5152,8 +5225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99173B9F-FA6E-408A-BCB9-8FBF9815597F}">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5167,26 +5240,26 @@
     <col min="7" max="7" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="61" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="62" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="62" t="s">
         <v>289</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="62" t="s">
         <v>290</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="62" t="s">
         <v>291</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5194,22 +5267,22 @@
       <c r="A2" s="31">
         <v>1</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="63" t="s">
         <v>299</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="64">
         <v>2020</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="65" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="34" t="s">
+      <c r="E2" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="66" t="s">
         <v>297</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="67" t="s">
         <v>304</v>
       </c>
     </row>
@@ -5217,22 +5290,22 @@
       <c r="A3" s="31">
         <v>2</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="63" t="s">
         <v>300</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="21">
         <v>2014</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="68" t="s">
         <v>301</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="69" t="s">
         <v>302</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="67" t="s">
         <v>66</v>
       </c>
     </row>
@@ -5240,22 +5313,22 @@
       <c r="A4" s="31">
         <v>3</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="63" t="s">
         <v>307</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="21">
         <v>2010</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="68" t="s">
         <v>305</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="69" t="s">
         <v>306</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="67" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5263,68 +5336,68 @@
       <c r="A5" s="31">
         <v>4</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="63" t="s">
         <v>308</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="21">
         <v>2024</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="68" t="s">
         <v>310</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="F5" s="56" t="s">
+      <c r="F5" s="69" t="s">
         <v>309</v>
       </c>
-      <c r="G5" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="G5" s="67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>5</v>
       </c>
-      <c r="B6" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="31">
-        <v>2018</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="63" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6" s="21">
+        <v>2021</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" s="69" t="s">
+        <v>312</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>6</v>
       </c>
-      <c r="B7" s="59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="31">
-        <v>2016</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="41" t="s">
+      <c r="B7" s="63" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" s="21">
+        <v>2009</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>315</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="F7" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="G7" s="67" t="s">
         <v>66</v>
       </c>
     </row>
@@ -5332,89 +5405,91 @@
       <c r="A8" s="31">
         <v>7</v>
       </c>
-      <c r="B8" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="35">
-        <v>2020</v>
-      </c>
-      <c r="D8" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>144</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="63" t="s">
+        <v>314</v>
+      </c>
+      <c r="C8" s="21">
+        <v>2009</v>
+      </c>
+      <c r="D8" s="70" t="s">
+        <v>317</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>298</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>318</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>8</v>
       </c>
-      <c r="B9" s="60" t="s">
-        <v>269</v>
-      </c>
-      <c r="C9" s="35">
-        <v>1996</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="G9" s="41" t="s">
+      <c r="B9" s="63" t="s">
+        <v>319</v>
+      </c>
+      <c r="C9" s="21">
+        <v>2010</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>321</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>320</v>
+      </c>
+      <c r="G9" s="67" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
+      <c r="A10" s="21">
         <v>9</v>
       </c>
-      <c r="B10" s="59" t="s">
-        <v>274</v>
-      </c>
-      <c r="C10" s="31">
-        <v>2015</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="63" t="s">
+        <v>322</v>
+      </c>
+      <c r="C10" s="21">
+        <v>2007</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>323</v>
+      </c>
+      <c r="E10" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="F10" s="69" t="s">
+        <v>324</v>
+      </c>
+      <c r="G10" s="67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>10</v>
       </c>
-      <c r="B11" s="59" t="s">
-        <v>274</v>
-      </c>
-      <c r="C11" s="31">
+      <c r="B11" s="63" t="s">
+        <v>319</v>
+      </c>
+      <c r="C11" s="21">
         <v>2014</v>
       </c>
-      <c r="D11" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="56" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="41" t="s">
+      <c r="D11" s="68" t="s">
+        <v>326</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="F11" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="G11" s="67" t="s">
         <v>66</v>
       </c>
     </row>
@@ -6518,7 +6593,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="31">
         <v>59</v>
       </c>
@@ -6650,7 +6725,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="31">
         <v>65</v>
       </c>
@@ -6968,7 +7043,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="31">
         <v>79</v>
       </c>
@@ -6991,7 +7066,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="31">
         <v>80</v>
       </c>
@@ -7014,7 +7089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="31">
         <v>81</v>
       </c>
@@ -7037,7 +7112,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="31">
         <v>82</v>
       </c>
@@ -7060,7 +7135,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="31">
         <v>83</v>
       </c>
@@ -7083,7 +7158,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="31">
         <v>84</v>
       </c>
@@ -7106,7 +7181,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="31">
         <v>85</v>
       </c>
@@ -7129,7 +7204,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="31">
         <v>86</v>
       </c>
@@ -7175,7 +7250,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="31">
         <v>88</v>
       </c>
@@ -7198,7 +7273,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="31">
         <v>89</v>
       </c>
@@ -7244,7 +7319,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="31">
         <v>91</v>
       </c>
@@ -7355,7 +7430,9 @@
     <hyperlink ref="D51" r:id="rId80" xr:uid="{F6B0FB81-C76D-4A84-9736-711E7168428A}"/>
     <hyperlink ref="D29" r:id="rId81" xr:uid="{F689FD28-4552-4D25-9308-D421BC8A9CD6}"/>
     <hyperlink ref="D5" r:id="rId82" xr:uid="{8EC10727-B27D-4E21-B65D-2E5D302FE622}"/>
+    <hyperlink ref="D9" r:id="rId83" xr:uid="{74AD30D2-3F30-468C-8863-A625EC79A43C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId84"/>
 </worksheet>
 </file>
</xml_diff>